<commit_message>
spajanje mob testova 10.12.2025
</commit_message>
<xml_diff>
--- a/testdata/execute.xlsx
+++ b/testdata/execute.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$12</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$13</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="80" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="122" uniqueCount="45">
   <si>
     <t>App</t>
   </si>
@@ -123,6 +123,48 @@
   </si>
   <si>
     <t>C95078</t>
+  </si>
+  <si>
+    <t>Product_Summary_Edit_Product_View[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>C95079</t>
+  </si>
+  <si>
+    <t>Domestic_Account_Filter_By_Type[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>C95080</t>
+  </si>
+  <si>
+    <t>Current_Accounts-Transactions-Filter-Multiple_Filter_[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>C95081</t>
+  </si>
+  <si>
+    <t>Currente_Accounts-Transactions-Filter-Clear-Filter[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>C95082</t>
+  </si>
+  <si>
+    <t>Product_Summary-Edit_Product_view-edit_name_of_account_[MOB_ANDROID]_1</t>
+  </si>
+  <si>
+    <t>C95083</t>
+  </si>
+  <si>
+    <t>Product_Summary-Edit_Product_view-edit_name_of_card_[MOB_ANDROID]_1</t>
+  </si>
+  <si>
+    <t>C95084</t>
+  </si>
+  <si>
+    <t>Product_Summary-Edit_Product_view-edit_name_of_deposit_[MOB_ANDROID]_1</t>
+  </si>
+  <si>
+    <t>C95085</t>
   </si>
 </sst>
 </file>
@@ -1095,10 +1137,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G13"/>
+  <dimension ref="A1:G20"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="C18" sqref="C18"/>
+      <selection activeCell="D22" sqref="D22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1373,8 +1415,148 @@
         <v>13</v>
       </c>
     </row>
+    <row r="14" spans="2:7">
+      <c r="B14" t="s">
+        <v>31</v>
+      </c>
+      <c r="C14" s="2" t="s">
+        <v>32</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E14" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F14" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G14" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="15" spans="2:7">
+      <c r="B15" t="s">
+        <v>33</v>
+      </c>
+      <c r="C15" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E15" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F15" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G15" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="16" spans="2:7">
+      <c r="B16" t="s">
+        <v>35</v>
+      </c>
+      <c r="C16" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E16" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G16" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="17" spans="2:7">
+      <c r="B17" t="s">
+        <v>37</v>
+      </c>
+      <c r="C17" s="2" t="s">
+        <v>38</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E17" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F17" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G17" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="18" spans="2:7">
+      <c r="B18" t="s">
+        <v>39</v>
+      </c>
+      <c r="C18" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E18" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F18" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G18" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="19" spans="2:7">
+      <c r="B19" t="s">
+        <v>41</v>
+      </c>
+      <c r="C19" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E19" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F19" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G19" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="20" spans="2:7">
+      <c r="B20" t="s">
+        <v>43</v>
+      </c>
+      <c r="C20" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E20" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F20" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G20" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G12" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G13" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Dobrodosli izadajice na Mobu
</commit_message>
<xml_diff>
--- a/testdata/execute.xlsx
+++ b/testdata/execute.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$24</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$25</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="175" uniqueCount="60">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="189" uniqueCount="64">
   <si>
     <t>App</t>
   </si>
@@ -210,6 +210,18 @@
   </si>
   <si>
     <t>C70802</t>
+  </si>
+  <si>
+    <t>Current_Domestic_Accounts-Transactions-Filter_By_Amount_Invalid_[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>C70803</t>
+  </si>
+  <si>
+    <t>Current_Domestic_Accounts-Transactions-List_[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>C70804</t>
   </si>
 </sst>
 </file>
@@ -1194,10 +1206,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G25"/>
+  <dimension ref="A1:G27"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="B29" sqref="B29"/>
+      <selection activeCell="E28" sqref="E28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1781,8 +1793,54 @@
         <v>13</v>
       </c>
     </row>
+    <row r="26" spans="1:7">
+      <c r="A26" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B26" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>61</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F26" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G26" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="27" spans="1:7">
+      <c r="A27" s="2" t="s">
+        <v>7</v>
+      </c>
+      <c r="B27" s="2" t="s">
+        <v>62</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F27" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G27" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G24" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G25" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="C$1:C$1048576">

</xml_diff>

<commit_message>
Domestic payment cance button
</commit_message>
<xml_diff>
--- a/testdata/execute.xlsx
+++ b/testdata/execute.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$35</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$38</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="262" uniqueCount="84">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="273" uniqueCount="86">
   <si>
     <t>App</t>
   </si>
@@ -282,6 +282,12 @@
   </si>
   <si>
     <t>C70813</t>
+  </si>
+  <si>
+    <t>Payments_Domestic_Payments_Cancel_Button_[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>C70814</t>
   </si>
 </sst>
 </file>
@@ -1267,10 +1273,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G38"/>
+  <dimension ref="A1:G39"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="D42" sqref="D42"/>
+      <selection activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -2061,7 +2067,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="35" spans="2:7">
+    <row r="35" spans="1:7">
+      <c r="A35" t="s">
+        <v>7</v>
+      </c>
       <c r="B35" t="s">
         <v>77</v>
       </c>
@@ -2081,7 +2090,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="36" spans="2:7">
+    <row r="36" spans="1:7">
+      <c r="A36" t="s">
+        <v>7</v>
+      </c>
       <c r="B36" s="5" t="s">
         <v>79</v>
       </c>
@@ -2101,7 +2113,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="37" customFormat="1" spans="2:7">
+    <row r="37" customFormat="1" spans="1:7">
+      <c r="A37" t="s">
+        <v>7</v>
+      </c>
       <c r="B37" s="5" t="s">
         <v>81</v>
       </c>
@@ -2121,7 +2136,10 @@
         <v>13</v>
       </c>
     </row>
-    <row r="38" spans="2:7">
+    <row r="38" spans="1:7">
+      <c r="A38" t="s">
+        <v>7</v>
+      </c>
       <c r="B38" s="5" t="s">
         <v>82</v>
       </c>
@@ -2141,17 +2159,40 @@
         <v>13</v>
       </c>
     </row>
+    <row r="39" spans="1:7">
+      <c r="A39" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" t="s">
+        <v>84</v>
+      </c>
+      <c r="C39" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="D39" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E39" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G39" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G35" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G38" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="C31:C36">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C38">
+  <conditionalFormatting sqref="C37:C39">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C30 C39:C1048576">
+  <conditionalFormatting sqref="C1:C30 C40:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="3"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Credit Card - filteri polovicno
</commit_message>
<xml_diff>
--- a/testdata/execute.xlsx
+++ b/testdata/execute.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="22188" windowHeight="9000"/>
+    <workbookView windowWidth="23040" windowHeight="10187"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$39</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$41</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="287" uniqueCount="90">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="93">
   <si>
     <t>App</t>
   </si>
@@ -300,6 +300,15 @@
   </si>
   <si>
     <t>C70816</t>
+  </si>
+  <si>
+    <t>Credit_cards-Transactions-Filter-Filter_By_Type_[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>Credit_cards-Transactions-Filter-Filter_By_Amount_[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>Credit_cards-Transactions-Filter-Filter_By_Amount_invalid_[MOB_ANDROID]</t>
   </si>
 </sst>
 </file>
@@ -1285,10 +1294,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G41"/>
+  <dimension ref="A1:G44"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="C43" sqref="C43"/>
+      <selection activeCell="B47" sqref="B47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -2240,18 +2249,96 @@
         <v>13</v>
       </c>
     </row>
+    <row r="42" spans="1:7">
+      <c r="A42" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" t="s">
+        <v>90</v>
+      </c>
+      <c r="C42" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D42" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E42" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F42" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G42" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="43" spans="1:7">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E43" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F43" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G43" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="44" spans="1:7">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>89</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E44" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F44" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G44" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G39" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G41" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
-  <conditionalFormatting sqref="C31:C36">
+  <conditionalFormatting sqref="C42">
+    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C43">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C37:C41">
+  <conditionalFormatting sqref="C44">
     <cfRule type="duplicateValues" dxfId="0" priority="1"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C30 C42:C1048576">
-    <cfRule type="duplicateValues" dxfId="0" priority="3"/>
+  <conditionalFormatting sqref="C31:C36">
+    <cfRule type="duplicateValues" dxfId="0" priority="5"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C37:C41">
+    <cfRule type="duplicateValues" dxfId="0" priority="4"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C30 C45:C1048576">
+    <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <headerFooter/>

</xml_diff>

<commit_message>
Izmena u testu Deposit list i u stepsu fji koja proverava da je ceo depozit clickable
</commit_message>
<xml_diff>
--- a/testdata/execute.xlsx
+++ b/testdata/execute.xlsx
@@ -4,13 +4,13 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="23040" windowHeight="10187"/>
+    <workbookView windowWidth="22188" windowHeight="9000"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$41</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$G$44</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="93">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="315" uniqueCount="95">
   <si>
     <t>App</t>
   </si>
@@ -309,6 +309,12 @@
   </si>
   <si>
     <t>Credit_cards-Transactions-Filter-Filter_By_Amount_invalid_[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>Product_Summary-Term_Deposit_List_[MOB_ANDROID]</t>
+  </si>
+  <si>
+    <t>C70817</t>
   </si>
 </sst>
 </file>
@@ -954,7 +960,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
@@ -962,7 +968,8 @@
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="49">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1294,10 +1301,10 @@
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:G44"/>
+  <dimension ref="A1:G45"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A26" workbookViewId="0">
-      <selection activeCell="B47" sqref="B47"/>
+    <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="E46" sqref="E46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9" defaultRowHeight="14.4" outlineLevelCol="6"/>
@@ -1928,10 +1935,10 @@
       </c>
     </row>
     <row r="28" spans="1:7">
-      <c r="A28" t="s">
-        <v>7</v>
-      </c>
-      <c r="B28" t="s">
+      <c r="A28" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" s="5" t="s">
         <v>64</v>
       </c>
       <c r="C28" s="2" t="s">
@@ -1951,10 +1958,10 @@
       </c>
     </row>
     <row r="29" spans="1:7">
-      <c r="A29" t="s">
-        <v>7</v>
-      </c>
-      <c r="B29" t="s">
+      <c r="A29" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" s="5" t="s">
         <v>66</v>
       </c>
       <c r="C29" s="2" t="s">
@@ -1974,10 +1981,10 @@
       </c>
     </row>
     <row r="30" spans="1:7">
-      <c r="A30" t="s">
-        <v>7</v>
-      </c>
-      <c r="B30" s="5" t="s">
+      <c r="A30" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" s="6" t="s">
         <v>68</v>
       </c>
       <c r="C30" s="2" t="s">
@@ -1997,10 +2004,10 @@
       </c>
     </row>
     <row r="31" customFormat="1" spans="1:7">
-      <c r="A31" t="s">
-        <v>7</v>
-      </c>
-      <c r="B31" s="5" t="s">
+      <c r="A31" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" s="6" t="s">
         <v>70</v>
       </c>
       <c r="C31" s="2" t="s">
@@ -2020,10 +2027,10 @@
       </c>
     </row>
     <row r="32" spans="1:7">
-      <c r="A32" t="s">
-        <v>7</v>
-      </c>
-      <c r="B32" t="s">
+      <c r="A32" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B32" s="5" t="s">
         <v>71</v>
       </c>
       <c r="C32" s="2" t="s">
@@ -2043,10 +2050,10 @@
       </c>
     </row>
     <row r="33" spans="1:7">
-      <c r="A33" t="s">
-        <v>7</v>
-      </c>
-      <c r="B33" t="s">
+      <c r="A33" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B33" s="5" t="s">
         <v>73</v>
       </c>
       <c r="C33" s="2" t="s">
@@ -2066,10 +2073,10 @@
       </c>
     </row>
     <row r="34" spans="1:7">
-      <c r="A34" t="s">
-        <v>7</v>
-      </c>
-      <c r="B34" t="s">
+      <c r="A34" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B34" s="5" t="s">
         <v>75</v>
       </c>
       <c r="C34" s="2" t="s">
@@ -2089,10 +2096,10 @@
       </c>
     </row>
     <row r="35" spans="1:7">
-      <c r="A35" t="s">
-        <v>7</v>
-      </c>
-      <c r="B35" t="s">
+      <c r="A35" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B35" s="5" t="s">
         <v>77</v>
       </c>
       <c r="C35" s="2" t="s">
@@ -2112,10 +2119,10 @@
       </c>
     </row>
     <row r="36" spans="1:7">
-      <c r="A36" t="s">
-        <v>7</v>
-      </c>
-      <c r="B36" s="5" t="s">
+      <c r="A36" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B36" s="6" t="s">
         <v>79</v>
       </c>
       <c r="C36" s="2" t="s">
@@ -2135,10 +2142,10 @@
       </c>
     </row>
     <row r="37" customFormat="1" spans="1:7">
-      <c r="A37" t="s">
-        <v>7</v>
-      </c>
-      <c r="B37" s="5" t="s">
+      <c r="A37" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B37" s="6" t="s">
         <v>81</v>
       </c>
       <c r="C37" s="2" t="s">
@@ -2158,10 +2165,10 @@
       </c>
     </row>
     <row r="38" spans="1:7">
-      <c r="A38" t="s">
-        <v>7</v>
-      </c>
-      <c r="B38" s="5" t="s">
+      <c r="A38" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B38" s="6" t="s">
         <v>82</v>
       </c>
       <c r="C38" s="2" t="s">
@@ -2181,10 +2188,10 @@
       </c>
     </row>
     <row r="39" spans="1:7">
-      <c r="A39" t="s">
-        <v>7</v>
-      </c>
-      <c r="B39" t="s">
+      <c r="A39" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B39" s="5" t="s">
         <v>84</v>
       </c>
       <c r="C39" s="2" t="s">
@@ -2204,10 +2211,10 @@
       </c>
     </row>
     <row r="40" spans="1:7">
-      <c r="A40" t="s">
-        <v>7</v>
-      </c>
-      <c r="B40" t="s">
+      <c r="A40" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B40" s="5" t="s">
         <v>86</v>
       </c>
       <c r="C40" s="2" t="s">
@@ -2227,10 +2234,10 @@
       </c>
     </row>
     <row r="41" spans="1:7">
-      <c r="A41" t="s">
-        <v>7</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="A41" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B41" s="5" t="s">
         <v>88</v>
       </c>
       <c r="C41" s="2" t="s">
@@ -2250,10 +2257,10 @@
       </c>
     </row>
     <row r="42" spans="1:7">
-      <c r="A42" t="s">
-        <v>7</v>
-      </c>
-      <c r="B42" t="s">
+      <c r="A42" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B42" s="5" t="s">
         <v>90</v>
       </c>
       <c r="C42" s="2" t="s">
@@ -2273,10 +2280,10 @@
       </c>
     </row>
     <row r="43" spans="1:7">
-      <c r="A43" t="s">
-        <v>7</v>
-      </c>
-      <c r="B43" t="s">
+      <c r="A43" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" s="5" t="s">
         <v>91</v>
       </c>
       <c r="C43" s="2" t="s">
@@ -2296,10 +2303,10 @@
       </c>
     </row>
     <row r="44" spans="1:7">
-      <c r="A44" t="s">
-        <v>7</v>
-      </c>
-      <c r="B44" t="s">
+      <c r="A44" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" s="5" t="s">
         <v>92</v>
       </c>
       <c r="C44" s="2" t="s">
@@ -2318,8 +2325,31 @@
         <v>13</v>
       </c>
     </row>
+    <row r="45" spans="1:7">
+      <c r="A45" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" s="5" t="s">
+        <v>93</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>10</v>
+      </c>
+      <c r="E45" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F45" s="2" t="s">
+        <v>12</v>
+      </c>
+      <c r="G45" s="2" t="s">
+        <v>13</v>
+      </c>
+    </row>
   </sheetData>
-  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G41" etc:filterBottomFollowUsedRange="0">
+  <autoFilter xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData" ref="A1:G44" etc:filterBottomFollowUsedRange="0">
     <extLst/>
   </autoFilter>
   <conditionalFormatting sqref="C42">
@@ -2328,16 +2358,16 @@
   <conditionalFormatting sqref="C43">
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C44">
-    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
-  </conditionalFormatting>
   <conditionalFormatting sqref="C31:C36">
     <cfRule type="duplicateValues" dxfId="0" priority="5"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="C37:C41">
     <cfRule type="duplicateValues" dxfId="0" priority="4"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="C1:C30 C45:C1048576">
+  <conditionalFormatting sqref="C44:C45">
+    <cfRule type="duplicateValues" dxfId="0" priority="1"/>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="C1:C30 C46:C1048576">
     <cfRule type="duplicateValues" dxfId="0" priority="6"/>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>